<commit_message>
fix logos for election
</commit_message>
<xml_diff>
--- a/db/uploads/3rd_octs_ga_coop.xlsx
+++ b/db/uploads/3rd_octs_ga_coop.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ansellgabrieldelayre/Sites/ga_system_octs/db/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9409D4FC-9601-8145-A0F8-7B9A56739DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B8474E-F69B-454E-98B0-B7DEED50C805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="920" windowWidth="24780" windowHeight="15500" xr2:uid="{C44A4133-3FA1-AB41-B6F5-B460161B5849}"/>
+    <workbookView xWindow="3460" yWindow="920" windowWidth="24780" windowHeight="15500" activeTab="1" xr2:uid="{C44A4133-3FA1-AB41-B6F5-B460161B5849}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="145">
   <si>
     <t>First Community Cooperative</t>
   </si>
@@ -476,7 +477,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -490,6 +494,19 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -499,7 +516,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -507,15 +524,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -850,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2BD7FD2-2C75-E242-A47B-BB105F852612}">
   <dimension ref="A1:C143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2439,4 +2477,782 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041EBE7B-C657-844E-97C8-864F1AB987AB}">
+  <dimension ref="A2:B96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="83.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.04003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.022</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B80" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B81" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B95" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B96" s="3">
+        <v>1.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>